<commit_message>
Activties - Single Activity Type
</commit_message>
<xml_diff>
--- a/readme/Decisions.xlsx
+++ b/readme/Decisions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\martynt.medallia\Documents\eligiblity-rule-helper-vue\readme\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\martynt.Medallia\Documents\eligiblity-rule-helper-vue\readme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F6D33A-8C29-4C5F-9439-711CBD9BB4BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBF2AEB5-6919-4CD6-96BB-2125CD0616EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5385" yWindow="-21720" windowWidth="38640" windowHeight="21240" xr2:uid="{48BAF3A2-41C2-4885-B9C2-F29876B92AB8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{48BAF3A2-41C2-4885-B9C2-F29876B92AB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -954,8 +954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EB7BD85-0B31-4842-A1FA-5FC6C6D2E822}">
   <dimension ref="A1:M119"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView tabSelected="1" topLeftCell="G119" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M34" sqref="M34:M119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>